<commit_message>
Add datasets download link
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tridinc/Projects/genex/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tridinc/Projects/genex/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -93,13 +93,16 @@
   </si>
   <si>
     <t>Size of training set (query)</t>
+  </si>
+  <si>
+    <t>Download datasets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +114,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,16 +144,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +484,7 @@
         <v>24</v>
       </c>
       <c r="F3">
-        <f>D3*E3*(E3-1)/2</f>
+        <f t="shared" ref="F3:F12" si="0">D3*E3*(E3-1)/2</f>
         <v>30084</v>
       </c>
     </row>
@@ -491,7 +505,7 @@
         <v>96</v>
       </c>
       <c r="F4">
-        <f>D4*E4*(E4-1)/2</f>
+        <f t="shared" si="0"/>
         <v>456000</v>
       </c>
     </row>
@@ -512,7 +526,7 @@
         <v>60</v>
       </c>
       <c r="F5">
-        <f>D5*E5*(E5-1)/2</f>
+        <f t="shared" si="0"/>
         <v>531000</v>
       </c>
     </row>
@@ -533,7 +547,7 @@
         <v>150</v>
       </c>
       <c r="F6">
-        <f>D6*E6*(E6-1)/2</f>
+        <f t="shared" si="0"/>
         <v>1676250</v>
       </c>
     </row>
@@ -554,7 +568,7 @@
         <v>131</v>
       </c>
       <c r="F7">
-        <f>D7*E7*(E7-1)/2</f>
+        <f t="shared" si="0"/>
         <v>14390350</v>
       </c>
     </row>
@@ -575,7 +589,7 @@
         <v>128</v>
       </c>
       <c r="F8">
-        <f>D8*E8*(E8-1)/2</f>
+        <f t="shared" si="0"/>
         <v>32512000</v>
       </c>
     </row>
@@ -596,7 +610,7 @@
         <v>152</v>
       </c>
       <c r="F9">
-        <f>D9*E9*(E9-1)/2</f>
+        <f t="shared" si="0"/>
         <v>70852824</v>
       </c>
     </row>
@@ -617,7 +631,7 @@
         <v>1092</v>
       </c>
       <c r="F10">
-        <f>D10*E10*(E10-1)/2</f>
+        <f t="shared" si="0"/>
         <v>183471288</v>
       </c>
     </row>
@@ -638,7 +652,7 @@
         <v>1024</v>
       </c>
       <c r="F11">
-        <f>D11*E11*(E11-1)/2</f>
+        <f t="shared" si="0"/>
         <v>1228254720</v>
       </c>
     </row>
@@ -659,14 +673,22 @@
         <v>1024</v>
       </c>
       <c r="F12">
-        <f>D12*E12*(E12-1)/2</f>
+        <f t="shared" si="0"/>
         <v>4313819136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A3:F12">
     <sortCondition ref="F1"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="A15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>